<commit_message>
Avances hasta el 08-06-2019
</commit_message>
<xml_diff>
--- a/ejemplo3.xlsx
+++ b/ejemplo3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INSPIRON\Documents\Sicee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\SiceeGIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7656"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -161,13 +161,13 @@
     <t>EE2</t>
   </si>
   <si>
-    <t>EE3</t>
-  </si>
-  <si>
-    <t>EE4</t>
-  </si>
-  <si>
     <t>02IE</t>
+  </si>
+  <si>
+    <t>EF1</t>
+  </si>
+  <si>
+    <t>EF2</t>
   </si>
 </sst>
 </file>
@@ -489,12 +489,12 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -552,12 +552,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -575,7 +575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -598,7 +598,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -621,7 +621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -644,7 +644,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -667,12 +667,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -690,7 +690,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -713,7 +713,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -730,13 +730,13 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Guardar cambios en bitácora de asistencia
</commit_message>
<xml_diff>
--- a/ejemplo3.xlsx
+++ b/ejemplo3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>DocenteEmpleado_id</t>
   </si>
@@ -155,12 +155,6 @@
     <t>ED4</t>
   </si>
   <si>
-    <t>EE1</t>
-  </si>
-  <si>
-    <t>EE2</t>
-  </si>
-  <si>
     <t>02IE</t>
   </si>
   <si>
@@ -168,6 +162,12 @@
   </si>
   <si>
     <t>EF2</t>
+  </si>
+  <si>
+    <t>EF3</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -486,276 +486,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="B1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>